<commit_message>
change main_controlDialog to buffered GetRequests ==> jalousie event data not jet correct displayed
</commit_message>
<xml_diff>
--- a/CPS_protokoll.xlsx
+++ b/CPS_protokoll.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Tabelle1" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
@@ -25,15 +25,17 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="248">
   <si>
     <t xml:space="preserve">Int[]</t>
   </si>
@@ -949,12 +951,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,25 +1369,25 @@
   </sheetPr>
   <dimension ref="2:35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,6 +1814,15 @@
       </c>
       <c r="L24" s="0" t="s">
         <v>136</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,10 +2130,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,7 +3193,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D75"/>
+  <autoFilter ref="A1:D73"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3207,7 +3218,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
bugfix display PBplatformControl @heater
</commit_message>
<xml_diff>
--- a/CPS_protokoll.xlsx
+++ b/CPS_protokoll.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frame" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="Tabelle1" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
@@ -26,16 +26,18 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -466,10 +468,10 @@
     <t xml:space="preserve">reserve</t>
   </si>
   <si>
-    <t xml:space="preserve">ctrl_manuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctrl_mauel_state</t>
+    <t xml:space="preserve">ctrl_manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ctrl_maual_state</t>
   </si>
   <si>
     <t xml:space="preserve">timeOnHour</t>
@@ -951,12 +953,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,25 +1371,24 @@
   </sheetPr>
   <dimension ref="2:35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.72959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.87244897959184"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,10 +2131,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,7 +3194,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D73"/>
+  <autoFilter ref="A1:D75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3217,9 +3218,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
commit test in branche interfaceWatchdogTime
</commit_message>
<xml_diff>
--- a/CPS_protokoll.xlsx
+++ b/CPS_protokoll.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Frame" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="JOB" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ID" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Tabelle1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="struktureIOdata" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
@@ -27,17 +27,19 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="249">
   <si>
     <t xml:space="preserve">Int[]</t>
   </si>
@@ -793,6 +795,9 @@
   </si>
   <si>
     <t xml:space="preserve">ID_drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -953,12 +958,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,18 +1382,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.72959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.87244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,10 +2138,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3194,7 +3201,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D75"/>
+  <autoFilter ref="A1:D73"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3211,14 +3218,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
update merge from local repo to remote "AutoHomeGUI" repo
</commit_message>
<xml_diff>
--- a/CPS_protokoll.xlsx
+++ b/CPS_protokoll.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Frame" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="JOB" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ID" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Tabelle1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="struktureIOdata" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
@@ -27,17 +27,19 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="249">
   <si>
     <t xml:space="preserve">Int[]</t>
   </si>
@@ -793,6 +795,9 @@
   </si>
   <si>
     <t xml:space="preserve">ID_drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -953,12 +958,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,18 +1382,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.72959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.87244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,10 +2138,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3194,7 +3201,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D75"/>
+  <autoFilter ref="A1:D73"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3211,14 +3218,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>